<commit_message>
Step on the bright side of PEP8, refactoring use of program data, add commitplan.txt
</commit_message>
<xml_diff>
--- a/man/Данные маркировки.xlsx
+++ b/man/Данные маркировки.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proj\MarkV\man\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A354DE2-54D4-4CAF-B3A3-D54F7EAE160A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175D5FB4-D20C-4317-81A5-59A418D240B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8952" yWindow="1272" windowWidth="18564" windowHeight="13932" tabRatio="1000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8220" yWindow="2760" windowWidth="17772" windowHeight="16620" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Счётчики" sheetId="6" r:id="rId1"/>
@@ -58,25 +58,20 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="СЭТ / ПР-3" guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="996" activeSheetId="1"/>
+    <customWorkbookView name="ПР-3 / СЭТ" guid="{14CB70C2-A070-40AE-B4D7-80C305813711}" includePrintSettings="0" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="996" activeSheetId="1"/>
     <customWorkbookView name="Обычное" guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="996" activeSheetId="8"/>
-    <customWorkbookView name="ПР-3 / СЭТ" guid="{14CB70C2-A070-40AE-B4D7-80C305813711}" includePrintSettings="0" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="996" activeSheetId="1"/>
-    <customWorkbookView name="СЭТ / ПР-3" guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="996" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2359" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2359" uniqueCount="829">
   <si>
     <t>Сечение</t>
   </si>
@@ -2546,9 +2541,6 @@
     <t>нов.</t>
   </si>
   <si>
-    <t>RS-485 ПР-3</t>
-  </si>
-  <si>
     <t>ПР-3:1</t>
   </si>
   <si>
@@ -2561,9 +2553,6 @@
     <t>ПР-3:5</t>
   </si>
   <si>
-    <t>RS-485 СЭТ1</t>
-  </si>
-  <si>
     <t>Wh:16</t>
   </si>
   <si>
@@ -2576,9 +2565,6 @@
     <t>Wh:18</t>
   </si>
   <si>
-    <t>RS-485 СЭТ2</t>
-  </si>
-  <si>
     <t>Wh:13</t>
   </si>
   <si>
@@ -2589,6 +2575,12 @@
   </si>
   <si>
     <t>XXXX-XXXX-XXXXX</t>
+  </si>
+  <si>
+    <t>СЭТ2</t>
+  </si>
+  <si>
+    <t>СЭТ1</t>
   </si>
 </sst>
 </file>
@@ -2747,7 +2739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2835,9 +2827,6 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3031,19 +3020,19 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3342,7 +3331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51" defaultRowHeight="56.85" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3441,7 +3430,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90" showPageBreaks="1" view="pageLayout">
+    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90" showPageBreaks="1" view="pageLayout">
       <pageMargins left="0.27559055118110237" right="0.27559055118110237" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
       <pageSetup paperSize="70" fitToWidth="3" fitToHeight="3" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
       <headerFooter>
@@ -3451,7 +3440,7 @@
       </headerFooter>
     </customSheetView>
     <customSheetView guid="{14CB70C2-A070-40AE-B4D7-80C305813711}" scale="90" showPageBreaks="1" view="pageLayout"/>
-    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90" showPageBreaks="1" view="pageLayout">
+    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90" showPageBreaks="1" view="pageLayout">
       <pageMargins left="0.27559055118110237" right="0.27559055118110237" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
       <pageSetup paperSize="70" fitToWidth="3" fitToHeight="3" pageOrder="overThenDown" orientation="portrait" r:id="rId2"/>
       <headerFooter>
@@ -3655,7 +3644,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90" showPageBreaks="1" view="pageLayout">
+    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90" showPageBreaks="1" view="pageLayout">
       <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
       <pageSetup paperSize="70" fitToWidth="3" fitToHeight="3" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
       <headerFooter>
@@ -3664,7 +3653,7 @@
       </headerFooter>
     </customSheetView>
     <customSheetView guid="{14CB70C2-A070-40AE-B4D7-80C305813711}" scale="90" showPageBreaks="1" view="pageLayout"/>
-    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90" showPageBreaks="1" view="pageLayout">
+    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90" showPageBreaks="1" view="pageLayout">
       <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
       <pageSetup paperSize="70" fitToWidth="3" fitToHeight="3" pageOrder="overThenDown" orientation="portrait" r:id="rId2"/>
       <headerFooter>
@@ -4428,7 +4417,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
+    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4438,7 +4427,7 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </customSheetView>
-    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
+    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -5183,14 +5172,14 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>815</v>
-      </c>
-      <c r="B28" s="43">
+        <v>60</v>
+      </c>
+      <c r="B28" s="42">
         <f>12*3-4</f>
         <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E28" s="2">
         <v>1.5</v>
@@ -5199,7 +5188,7 @@
         <v>39</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
@@ -5212,7 +5201,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>2</v>
@@ -5232,7 +5221,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>2</v>
@@ -5246,22 +5235,22 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B31" s="42">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="26" t="s">
         <v>820</v>
-      </c>
-      <c r="B31" s="43">
-        <v>10</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>822</v>
       </c>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -5274,7 +5263,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>2</v>
@@ -5294,7 +5283,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>2</v>
@@ -5308,13 +5297,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
-        <v>825</v>
-      </c>
-      <c r="B34" s="43">
+        <v>827</v>
+      </c>
+      <c r="B34" s="42">
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>2</v>
@@ -5323,7 +5312,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -5336,7 +5325,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>2</v>
@@ -5356,7 +5345,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>2</v>
@@ -5370,9 +5359,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
+    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5380,9 +5369,9 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </customSheetView>
-    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
+    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -5402,7 +5391,7 @@
   <sheetPr codeName="Лист3">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:J178"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -5557,7 +5546,7 @@
         <v>28</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>2</v>
@@ -7264,348 +7253,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A69"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A70"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A77"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A78"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A80"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106"/>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107"/>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109"/>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110"/>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111"/>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121"/>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123"/>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127"/>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A150"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A158"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A159"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A167"/>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170"/>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171"/>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A174"/>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175"/>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A177"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:J67" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <customSheetViews>
-    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90" showAutoFilter="1">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90" filter="1" showAutoFilter="1">
+      <pane xSplit="1" ySplit="6" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:K113" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+      <autoFilter ref="A1:K113" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <filterColumn colId="1">
+          <customFilters>
+            <customFilter val="*СЭТ"/>
+          </customFilters>
+        </filterColumn>
+        <filterColumn colId="2">
+          <customFilters>
+            <customFilter val="*ПР-3"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
     </customSheetView>
     <customSheetView guid="{14CB70C2-A070-40AE-B4D7-80C305813711}" scale="90" filter="1" showAutoFilter="1">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -7623,40 +7290,29 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90" filter="1" showAutoFilter="1">
-      <pane xSplit="1" ySplit="6" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight"/>
+    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90" showAutoFilter="1">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:K113" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <filterColumn colId="1">
-          <customFilters>
-            <customFilter val="*СЭТ"/>
-          </customFilters>
-        </filterColumn>
-        <filterColumn colId="2">
-          <customFilters>
-            <customFilter val="*ПР-3"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="A1:K113" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="A179:A1048576 A1:A52 A55">
-    <cfRule type="duplicateValues" dxfId="22" priority="17"/>
-    <cfRule type="beginsWith" dxfId="21" priority="18" operator="beginsWith" text="Сущ.">
-      <formula>LEFT(A1,LEN("Сущ."))="Сущ."</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54">
-    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
-    <cfRule type="beginsWith" dxfId="19" priority="4" operator="beginsWith" text="Сущ.">
+    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
+    <cfRule type="beginsWith" dxfId="21" priority="4" operator="beginsWith" text="Сущ.">
       <formula>LEFT(A53,LEN("Сущ."))="Сущ."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A67">
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="×">
+    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="×">
       <formula>NOT(ISERROR(SEARCH("×",A56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:A1048576 A1:A52 A55">
+    <cfRule type="duplicateValues" dxfId="19" priority="85"/>
+    <cfRule type="beginsWith" dxfId="18" priority="86" operator="beginsWith" text="Сущ.">
+      <formula>LEFT(A1,LEN("Сущ."))="Сущ."</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -7677,9 +7333,9 @@
   <sheetPr codeName="Лист4">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9170,7 +8826,7 @@
       <c r="A106" t="s">
         <v>803</v>
       </c>
-      <c r="B106" s="39">
+      <c r="B106" s="2">
         <v>1075</v>
       </c>
       <c r="C106" s="36" t="s">
@@ -9187,7 +8843,7 @@
       <c r="A107" t="s">
         <v>803</v>
       </c>
-      <c r="B107" s="39">
+      <c r="B107" s="2">
         <v>1076</v>
       </c>
       <c r="C107" s="36" t="s">
@@ -9204,7 +8860,7 @@
       <c r="A108" t="s">
         <v>803</v>
       </c>
-      <c r="B108" s="39">
+      <c r="B108" s="2">
         <v>1077</v>
       </c>
       <c r="C108" s="36" t="s">
@@ -9221,7 +8877,7 @@
       <c r="A109" t="s">
         <v>803</v>
       </c>
-      <c r="B109" s="39">
+      <c r="B109" s="2">
         <v>1078</v>
       </c>
       <c r="C109" s="36" t="s">
@@ -9238,7 +8894,7 @@
       <c r="A110" t="s">
         <v>803</v>
       </c>
-      <c r="B110" s="39">
+      <c r="B110" s="2">
         <v>1079</v>
       </c>
       <c r="C110" s="36" t="s">
@@ -9255,7 +8911,7 @@
       <c r="A111" t="s">
         <v>803</v>
       </c>
-      <c r="B111" s="39">
+      <c r="B111" s="2">
         <v>1080</v>
       </c>
       <c r="C111" s="36" t="s">
@@ -9272,7 +8928,7 @@
       <c r="A112" t="s">
         <v>803</v>
       </c>
-      <c r="B112" s="39">
+      <c r="B112" s="2">
         <v>1081</v>
       </c>
       <c r="C112" s="36" t="s">
@@ -9289,7 +8945,7 @@
       <c r="A113" t="s">
         <v>803</v>
       </c>
-      <c r="B113" s="39">
+      <c r="B113" s="2">
         <v>1082</v>
       </c>
       <c r="C113" s="36" t="s">
@@ -9306,7 +8962,7 @@
       <c r="A114" t="s">
         <v>803</v>
       </c>
-      <c r="B114" s="39">
+      <c r="B114" s="2">
         <v>1083</v>
       </c>
       <c r="C114" s="36" t="s">
@@ -9323,7 +8979,7 @@
       <c r="A115" t="s">
         <v>803</v>
       </c>
-      <c r="B115" s="39">
+      <c r="B115" s="2">
         <v>1084</v>
       </c>
       <c r="C115" s="36" t="s">
@@ -9340,7 +8996,7 @@
       <c r="A116" t="s">
         <v>804</v>
       </c>
-      <c r="B116" s="39">
+      <c r="B116" s="2">
         <v>4030</v>
       </c>
       <c r="C116" s="36" t="s">
@@ -9357,7 +9013,7 @@
       <c r="A117" t="s">
         <v>804</v>
       </c>
-      <c r="B117" s="39">
+      <c r="B117" s="2">
         <v>4031</v>
       </c>
       <c r="C117" s="36" t="s">
@@ -9374,7 +9030,7 @@
       <c r="A118" t="s">
         <v>804</v>
       </c>
-      <c r="B118" s="39">
+      <c r="B118" s="2">
         <v>4032</v>
       </c>
       <c r="C118" s="36" t="s">
@@ -9391,7 +9047,7 @@
       <c r="A119" t="s">
         <v>804</v>
       </c>
-      <c r="B119" s="39">
+      <c r="B119" s="2">
         <v>4033</v>
       </c>
       <c r="C119" s="36" t="s">
@@ -9408,7 +9064,7 @@
       <c r="A120" t="s">
         <v>804</v>
       </c>
-      <c r="B120" s="39">
+      <c r="B120" s="2">
         <v>4040</v>
       </c>
       <c r="C120" s="36" t="s">
@@ -9425,7 +9081,7 @@
       <c r="A121" t="s">
         <v>804</v>
       </c>
-      <c r="B121" s="39">
+      <c r="B121" s="2">
         <v>4041</v>
       </c>
       <c r="C121" s="36" t="s">
@@ -9442,7 +9098,7 @@
       <c r="A122" t="s">
         <v>804</v>
       </c>
-      <c r="B122" s="39">
+      <c r="B122" s="2">
         <v>4034</v>
       </c>
       <c r="C122" s="36" t="s">
@@ -9459,7 +9115,7 @@
       <c r="A123" t="s">
         <v>804</v>
       </c>
-      <c r="B123" s="39">
+      <c r="B123" s="2">
         <v>4035</v>
       </c>
       <c r="C123" s="36" t="s">
@@ -9476,7 +9132,7 @@
       <c r="A124" t="s">
         <v>804</v>
       </c>
-      <c r="B124" s="39">
+      <c r="B124" s="2">
         <v>4036</v>
       </c>
       <c r="C124" s="36" t="s">
@@ -9493,7 +9149,7 @@
       <c r="A125" t="s">
         <v>804</v>
       </c>
-      <c r="B125" s="39">
+      <c r="B125" s="2">
         <v>4037</v>
       </c>
       <c r="C125" s="36" t="s">
@@ -9510,7 +9166,7 @@
       <c r="A126" t="s">
         <v>805</v>
       </c>
-      <c r="B126" s="39">
+      <c r="B126" s="2">
         <v>4038</v>
       </c>
       <c r="C126" s="36" t="s">
@@ -9527,7 +9183,7 @@
       <c r="A127" t="s">
         <v>805</v>
       </c>
-      <c r="B127" s="39">
+      <c r="B127" s="2">
         <v>4039</v>
       </c>
       <c r="C127" s="36" t="s">
@@ -9541,509 +9197,503 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="41" t="s">
+      <c r="A128" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B128" s="41">
+      <c r="B128" s="40">
         <v>2001</v>
       </c>
-      <c r="C128" s="41" t="s">
+      <c r="C128" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D128" s="41" t="s">
+      <c r="D128" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="41" t="s">
+      <c r="A129" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B129" s="41">
+      <c r="B129" s="40">
         <v>200</v>
       </c>
-      <c r="C129" s="41" t="s">
+      <c r="C129" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="D129" s="41" t="s">
+      <c r="D129" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="41" t="s">
+      <c r="A130" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B130" s="41">
+      <c r="B130" s="40">
         <v>2002</v>
       </c>
-      <c r="C130" s="41" t="s">
+      <c r="C130" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="D130" s="41" t="s">
+      <c r="D130" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="41" t="s">
+      <c r="A131" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B131" s="41">
+      <c r="B131" s="40">
         <v>200</v>
       </c>
-      <c r="C131" s="41" t="s">
+      <c r="C131" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="D131" s="41" t="s">
+      <c r="D131" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="41" t="s">
+      <c r="A132" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B132" s="41">
+      <c r="B132" s="40">
         <v>2003</v>
       </c>
-      <c r="C132" s="41" t="s">
+      <c r="C132" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="D132" s="41" t="s">
+      <c r="D132" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="41" t="s">
+      <c r="A133" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B133" s="41">
+      <c r="B133" s="40">
         <v>200</v>
       </c>
-      <c r="C133" s="41" t="s">
+      <c r="C133" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="D133" s="41" t="s">
+      <c r="D133" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" s="41" t="s">
+      <c r="A134" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B134" s="41">
+      <c r="B134" s="40">
         <v>2004</v>
       </c>
-      <c r="C134" s="41" t="s">
+      <c r="C134" s="40" t="s">
         <v>383</v>
       </c>
-      <c r="D134" s="41" t="s">
+      <c r="D134" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" s="41" t="s">
+      <c r="A135" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B135" s="41">
+      <c r="B135" s="40">
         <v>200</v>
       </c>
-      <c r="C135" s="41" t="s">
+      <c r="C135" s="40" t="s">
         <v>308</v>
       </c>
-      <c r="D135" s="41" t="s">
+      <c r="D135" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" s="41" t="s">
+      <c r="A136" s="40" t="s">
         <v>370</v>
       </c>
-      <c r="B136" s="41">
+      <c r="B136" s="40">
         <v>2005</v>
       </c>
-      <c r="C136" s="41" t="s">
+      <c r="C136" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="D136" s="41" t="s">
+      <c r="D136" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="41" t="s">
+      <c r="A137" s="40" t="s">
         <v>370</v>
       </c>
-      <c r="B137" s="41">
+      <c r="B137" s="40">
         <v>200</v>
       </c>
-      <c r="C137" s="41" t="s">
+      <c r="C137" s="40" t="s">
         <v>384</v>
       </c>
-      <c r="D137" s="41" t="s">
+      <c r="D137" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" s="41" t="s">
+      <c r="A138" s="40" t="s">
         <v>371</v>
       </c>
-      <c r="B138" s="41">
+      <c r="B138" s="40">
         <v>2006</v>
       </c>
-      <c r="C138" s="41" t="s">
+      <c r="C138" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="D138" s="41" t="s">
+      <c r="D138" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="41" t="s">
+      <c r="A139" s="40" t="s">
         <v>371</v>
       </c>
-      <c r="B139" s="41">
+      <c r="B139" s="40">
         <v>200</v>
       </c>
-      <c r="C139" s="41" t="s">
+      <c r="C139" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="D139" s="41" t="s">
+      <c r="D139" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" s="41" t="s">
+      <c r="A140" s="40" t="s">
         <v>372</v>
       </c>
-      <c r="B140" s="41">
+      <c r="B140" s="40">
         <v>2007</v>
       </c>
-      <c r="C140" s="41" t="s">
+      <c r="C140" s="40" t="s">
         <v>385</v>
       </c>
-      <c r="D140" s="41" t="s">
+      <c r="D140" s="40" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" s="41" t="s">
+      <c r="A141" s="40" t="s">
         <v>372</v>
       </c>
-      <c r="B141" s="41">
+      <c r="B141" s="40">
         <v>200</v>
       </c>
-      <c r="C141" s="41" t="s">
+      <c r="C141" s="40" t="s">
         <v>315</v>
       </c>
-      <c r="D141" s="41" t="s">
+      <c r="D141" s="40" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" s="41" t="s">
+      <c r="A142" s="40" t="s">
         <v>373</v>
       </c>
-      <c r="B142" s="41">
+      <c r="B142" s="40">
         <v>2008</v>
       </c>
-      <c r="C142" s="41" t="s">
+      <c r="C142" s="40" t="s">
         <v>316</v>
       </c>
-      <c r="D142" s="41" t="s">
+      <c r="D142" s="40" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" s="41" t="s">
+      <c r="A143" s="40" t="s">
         <v>373</v>
       </c>
-      <c r="B143" s="41">
+      <c r="B143" s="40">
         <v>200</v>
       </c>
-      <c r="C143" s="41" t="s">
+      <c r="C143" s="40" t="s">
         <v>386</v>
       </c>
-      <c r="D143" s="41" t="s">
+      <c r="D143" s="40" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" s="41" t="s">
+      <c r="A144" s="40" t="s">
         <v>374</v>
       </c>
-      <c r="B144" s="41">
+      <c r="B144" s="40">
         <v>2009</v>
       </c>
-      <c r="C144" s="41" t="s">
+      <c r="C144" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="D144" s="41" t="s">
+      <c r="D144" s="40" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A145" s="41" t="s">
+      <c r="A145" s="40" t="s">
         <v>374</v>
       </c>
-      <c r="B145" s="41">
+      <c r="B145" s="40">
         <v>200</v>
       </c>
-      <c r="C145" s="41" t="s">
+      <c r="C145" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="D145" s="41" t="s">
+      <c r="D145" s="40" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" s="41" t="s">
+      <c r="A146" s="40" t="s">
         <v>375</v>
       </c>
-      <c r="B146" s="41">
+      <c r="B146" s="40">
         <v>2010</v>
       </c>
-      <c r="C146" s="41" t="s">
+      <c r="C146" s="40" t="s">
         <v>481</v>
       </c>
-      <c r="D146" s="41" t="s">
+      <c r="D146" s="40" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" s="41" t="s">
+      <c r="A147" s="40" t="s">
         <v>375</v>
       </c>
-      <c r="B147" s="41">
+      <c r="B147" s="40">
         <v>200</v>
       </c>
-      <c r="C147" s="41" t="s">
+      <c r="C147" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="D147" s="41" t="s">
+      <c r="D147" s="40" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" s="41" t="s">
+      <c r="A148" s="40" t="s">
         <v>377</v>
       </c>
-      <c r="B148" s="41">
+      <c r="B148" s="40">
         <v>6000</v>
       </c>
-      <c r="C148" s="41" t="s">
+      <c r="C148" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="D148" s="41" t="s">
+      <c r="D148" s="40" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" s="41" t="s">
+      <c r="A149" s="40" t="s">
         <v>377</v>
       </c>
-      <c r="B149" s="41">
+      <c r="B149" s="40">
         <v>202</v>
       </c>
-      <c r="C149" s="41" t="s">
+      <c r="C149" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D149" s="42" t="s">
+      <c r="D149" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" s="41" t="s">
+      <c r="A150" s="40" t="s">
         <v>377</v>
       </c>
-      <c r="B150" s="41">
+      <c r="B150" s="40">
         <v>6001</v>
       </c>
-      <c r="C150" s="41" t="s">
+      <c r="C150" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="D150" s="41" t="s">
+      <c r="D150" s="40" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" s="41" t="s">
+      <c r="A151" s="40" t="s">
         <v>378</v>
       </c>
-      <c r="B151" s="41">
+      <c r="B151" s="40">
         <v>6002</v>
       </c>
-      <c r="C151" s="41" t="s">
+      <c r="C151" s="40" t="s">
         <v>396</v>
       </c>
-      <c r="D151" s="41" t="s">
+      <c r="D151" s="40" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" s="41" t="s">
+      <c r="A152" s="40" t="s">
         <v>378</v>
       </c>
-      <c r="B152" s="41">
+      <c r="B152" s="40">
         <v>202</v>
       </c>
-      <c r="C152" s="41" t="s">
+      <c r="C152" s="40" t="s">
         <v>397</v>
       </c>
-      <c r="D152" s="42" t="s">
+      <c r="D152" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A153" s="41" t="s">
+      <c r="A153" s="40" t="s">
         <v>378</v>
       </c>
-      <c r="B153" s="41">
+      <c r="B153" s="40">
         <v>6003</v>
       </c>
-      <c r="C153" s="41" t="s">
+      <c r="C153" s="40" t="s">
         <v>398</v>
       </c>
-      <c r="D153" s="41" t="s">
+      <c r="D153" s="40" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" s="41" t="s">
+      <c r="A154" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="B154" s="41">
+      <c r="B154" s="40">
         <v>6004</v>
       </c>
-      <c r="C154" s="41" t="s">
+      <c r="C154" s="40" t="s">
         <v>399</v>
       </c>
-      <c r="D154" s="41" t="s">
+      <c r="D154" s="40" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" s="41" t="s">
+      <c r="A155" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="B155" s="41">
+      <c r="B155" s="40">
         <v>202</v>
       </c>
-      <c r="C155" s="41" t="s">
+      <c r="C155" s="40" t="s">
         <v>400</v>
       </c>
-      <c r="D155" s="42" t="s">
+      <c r="D155" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" s="41" t="s">
+      <c r="A156" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="B156" s="41">
+      <c r="B156" s="40">
         <v>6005</v>
       </c>
-      <c r="C156" s="41" t="s">
+      <c r="C156" s="40" t="s">
         <v>401</v>
       </c>
-      <c r="D156" s="41" t="s">
+      <c r="D156" s="40" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" s="41" t="s">
+      <c r="A157" s="40" t="s">
         <v>467</v>
       </c>
-      <c r="B157" s="41">
+      <c r="B157" s="40">
         <v>6006</v>
       </c>
-      <c r="C157" s="41" t="s">
+      <c r="C157" s="40" t="s">
         <v>402</v>
       </c>
-      <c r="D157" s="41" t="s">
+      <c r="D157" s="40" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A158" s="41" t="s">
+      <c r="A158" s="40" t="s">
         <v>467</v>
       </c>
-      <c r="B158" s="41">
+      <c r="B158" s="40">
         <v>202</v>
       </c>
-      <c r="C158" s="41" t="s">
+      <c r="C158" s="40" t="s">
         <v>403</v>
       </c>
-      <c r="D158" s="42" t="s">
+      <c r="D158" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" s="41" t="s">
+      <c r="A159" s="40" t="s">
         <v>467</v>
       </c>
-      <c r="B159" s="41">
+      <c r="B159" s="40">
         <v>6007</v>
       </c>
-      <c r="C159" s="41" t="s">
+      <c r="C159" s="40" t="s">
         <v>404</v>
       </c>
-      <c r="D159" s="41" t="s">
+      <c r="D159" s="40" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A160" s="41" t="s">
+      <c r="A160" s="40" t="s">
         <v>469</v>
       </c>
-      <c r="B160" s="41">
+      <c r="B160" s="40">
         <v>6008</v>
       </c>
-      <c r="C160" s="41" t="s">
+      <c r="C160" s="40" t="s">
         <v>405</v>
       </c>
-      <c r="D160" s="41" t="s">
+      <c r="D160" s="40" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A161" s="41" t="s">
+      <c r="A161" s="40" t="s">
         <v>469</v>
       </c>
-      <c r="B161" s="41">
+      <c r="B161" s="40">
         <v>202</v>
       </c>
-      <c r="C161" s="41" t="s">
+      <c r="C161" s="40" t="s">
         <v>406</v>
       </c>
-      <c r="D161" s="42" t="s">
+      <c r="D161" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" s="41" t="s">
+      <c r="A162" s="40" t="s">
         <v>469</v>
       </c>
-      <c r="B162" s="41">
+      <c r="B162" s="40">
         <v>6009</v>
       </c>
-      <c r="C162" s="41" t="s">
+      <c r="C162" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="D162" s="41" t="s">
+      <c r="D162" s="40" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" s="41"/>
-      <c r="B163" s="41"/>
-      <c r="C163" s="41"/>
-      <c r="D163" s="41"/>
-    </row>
   </sheetData>
-  <sortState ref="A343:D381">
-    <sortCondition ref="A343:A381"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A329:D367">
+    <sortCondition ref="A329:A367"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
+    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:C10"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -10051,9 +9701,9 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7:C10"/>
     </customSheetView>
-    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
+    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:C10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -10619,9 +10269,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
+    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -10629,9 +10279,9 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </customSheetView>
-    <customSheetView guid="{2C0EDEAF-9AA9-45F7-88FB-A8CB43F0DBAB}" scale="90">
+    <customSheetView guid="{E0170134-1D35-4BDE-8F6F-DD0BDCE5836C}" scale="90">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -10669,42 +10319,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>611</v>
       </c>
       <c r="C1" s="37" t="s">
         <v>800</v>
       </c>
       <c r="D1" s="37"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>811</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="43" t="s">
         <v>810</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="43" t="s">
         <v>610</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="43" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="40" t="s">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="39" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>812</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>